<commit_message>
Se agregan registros a la base de datos para mejorar las consultas
</commit_message>
<xml_diff>
--- a/Documentacion/Sustentacion marzo 2017/Observaciones del audio.xlsx
+++ b/Documentacion/Sustentacion marzo 2017/Observaciones del audio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>acuerdo de nivel de servicio</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">respecto a la creacion de placas y sticker </t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -414,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,6 +501,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>

</xml_diff>